<commit_message>
twice as many sample items, data plots look nice
</commit_message>
<xml_diff>
--- a/netflix_films.xlsx
+++ b/netflix_films.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="183">
   <si>
     <t>Netflix_id</t>
   </si>
@@ -50,6 +50,147 @@
     <t>IMDB_id</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
     <t>60037627</t>
   </si>
   <si>
@@ -59,39 +200,9 @@
     <t>60036691</t>
   </si>
   <si>
-    <t>80025678</t>
-  </si>
-  <si>
-    <t>70177083</t>
-  </si>
-  <si>
-    <t>1e+08</t>
-  </si>
-  <si>
-    <t>10000000</t>
-  </si>
-  <si>
-    <t>abcdefgh</t>
-  </si>
-  <si>
-    <t>80144588</t>
-  </si>
-  <si>
     <t>80037759</t>
   </si>
   <si>
-    <t>70184207</t>
-  </si>
-  <si>
-    <t>80025384</t>
-  </si>
-  <si>
-    <t>80000770</t>
-  </si>
-  <si>
-    <t>80107369</t>
-  </si>
-  <si>
     <t>80097003</t>
   </si>
   <si>
@@ -101,37 +212,25 @@
     <t>80091741</t>
   </si>
   <si>
-    <t>80117470</t>
-  </si>
-  <si>
-    <t>80053653</t>
-  </si>
-  <si>
     <t>939827</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>28</t>
+    <t>80168188</t>
+  </si>
+  <si>
+    <t>70049392</t>
+  </si>
+  <si>
+    <t>80088567</t>
+  </si>
+  <si>
+    <t>70300205</t>
+  </si>
+  <si>
+    <t>70208248</t>
+  </si>
+  <si>
+    <t>60029157</t>
   </si>
   <si>
     <t>The Manchurian Candidate</t>
@@ -158,6 +257,24 @@
     <t>Scream</t>
   </si>
   <si>
+    <t>Chasing Coral</t>
+  </si>
+  <si>
+    <t>The Astronaut Farmer</t>
+  </si>
+  <si>
+    <t>Captain America: Civil War</t>
+  </si>
+  <si>
+    <t>The Babadook</t>
+  </si>
+  <si>
+    <t>J. Edgar</t>
+  </si>
+  <si>
+    <t>Pirates of the Caribbean: The Curse of the Black Pearl</t>
+  </si>
+  <si>
     <t>2004</t>
   </si>
   <si>
@@ -179,6 +296,15 @@
     <t>1996</t>
   </si>
   <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
     <t>R</t>
   </si>
   <si>
@@ -191,6 +317,12 @@
     <t>PG-13</t>
   </si>
   <si>
+    <t>TV-PG</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
     <t>2h 9m</t>
   </si>
   <si>
@@ -212,6 +344,24 @@
     <t>1h 51m</t>
   </si>
   <si>
+    <t>1h 29m</t>
+  </si>
+  <si>
+    <t>1h 44m</t>
+  </si>
+  <si>
+    <t>2h 28m</t>
+  </si>
+  <si>
+    <t>1h 33m</t>
+  </si>
+  <si>
+    <t>2h 16m</t>
+  </si>
+  <si>
+    <t>2h 23m</t>
+  </si>
+  <si>
     <t>Two U.S. soldiers in the first Gulf War are programmed to rebel once they return home. Several years later, one becomes a vice presidential candidate.</t>
   </si>
   <si>
@@ -236,6 +386,24 @@
     <t>A year after her mother's brutal murder, a high school girl and her friends are stalked by a serial killer who's obsessed with horror movies.</t>
   </si>
   <si>
+    <t>Divers, scientists and photographers around the world mount an epic underwater campaign to document the disappearance of coral reefs.</t>
+  </si>
+  <si>
+    <t>A NASA astronaut in training must shelve his dream to save his family's farm -- until one day, he decides to build a homegrown rocket in his barn.</t>
+  </si>
+  <si>
+    <t>It's Avengers vs. Avengers when Captain America fights to keep his superhero friends independent, while his pal Iron Man supports government control.</t>
+  </si>
+  <si>
+    <t>Sam's frequent tantrums turn sinister when a creepy children's book mysteriously appears in his room, and he asks his mother, "Do you want to die?"</t>
+  </si>
+  <si>
+    <t>This biopic profiles J. Edgar Hoover, who pushed the envelope professionally and led a complex personal life over nearly 50 years as head of the FBI.</t>
+  </si>
+  <si>
+    <t>When a young swain recruits pirate Capt. Jack Sparrow to help rescue a maiden from rival buccaneers, he finds he's up against supernatural forces.</t>
+  </si>
+  <si>
     <t>Thrillers, Psychological Thrillers, Political Thrillers</t>
   </si>
   <si>
@@ -260,6 +428,24 @@
     <t>Cult Movies, Cult Horror Movies, Horror Movies, Slasher and Serial Killer Movies, Teen Screams</t>
   </si>
   <si>
+    <t>Documentaries, Science &amp; Nature Docs</t>
+  </si>
+  <si>
+    <t>Dramas, Independent Dramas, Independent Movies, Sci-Fi &amp; Fantasy, Sci-Fi Dramas</t>
+  </si>
+  <si>
+    <t>Action &amp; Adventure, Adventures, Comic Book and Superhero Movies, Sci-Fi &amp; Fantasy, Action Sci-Fi &amp; Fantasy, Sci-Fi Adventure</t>
+  </si>
+  <si>
+    <t>Thrillers, Independent Thrillers, Psychological Thrillers, Supernatural Thrillers, Horror Movies, Supernatural Horror Movies, Independent Movies, Australian Movies</t>
+  </si>
+  <si>
+    <t>Dramas, Biographical Dramas, Crime Dramas, Dramas based on Real Life, 20th Century Period Pieces, Political Dramas</t>
+  </si>
+  <si>
+    <t>Action &amp; Adventure, Action Comedies, Adventures, Disney, Comedies</t>
+  </si>
+  <si>
     <t>Jonathan Demme</t>
   </si>
   <si>
@@ -284,6 +470,24 @@
     <t>Wes Craven</t>
   </si>
   <si>
+    <t>Jeff Orlowski</t>
+  </si>
+  <si>
+    <t>Michael Polish</t>
+  </si>
+  <si>
+    <t>Anthony Russo, Joe Russo</t>
+  </si>
+  <si>
+    <t>Jennifer Kent</t>
+  </si>
+  <si>
+    <t>Clint Eastwood</t>
+  </si>
+  <si>
+    <t>Gore Verbinski</t>
+  </si>
+  <si>
     <t>Denzel Washington, Meryl Streep, Liev Schreiber</t>
   </si>
   <si>
@@ -302,6 +506,21 @@
     <t>Neve Campbell, David Arquette, Courteney Cox</t>
   </si>
   <si>
+    <t>Billy Bob Thornton, Virginia Madsen, Bruce Dern</t>
+  </si>
+  <si>
+    <t>Chris Evans, Robert Downey Jr., Scarlett Johansson</t>
+  </si>
+  <si>
+    <t>Essie Davis, Noah Wiseman, Hayley McElhinney</t>
+  </si>
+  <si>
+    <t>Leonardo DiCaprio, Naomi Watts, Judi Dench</t>
+  </si>
+  <si>
+    <t>Johnny Depp, Geoffrey Rush, Orlando Bloom</t>
+  </si>
+  <si>
     <t>tt0368008</t>
   </si>
   <si>
@@ -324,6 +543,24 @@
   </si>
   <si>
     <t>tt0117571</t>
+  </si>
+  <si>
+    <t>tt6333054</t>
+  </si>
+  <si>
+    <t>tt0469263</t>
+  </si>
+  <si>
+    <t>tt3498820</t>
+  </si>
+  <si>
+    <t>tt2321549</t>
+  </si>
+  <si>
+    <t>tt1616195</t>
+  </si>
+  <si>
+    <t>tt0325980</t>
   </si>
 </sst>
 </file>
@@ -1237,32 +1474,32 @@
       <c r="A22" t="s">
         <v>32</v>
       </c>
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H22" t="s">
-        <v>74</v>
-      </c>
-      <c r="I22" t="s">
-        <v>82</v>
-      </c>
-      <c r="J22" t="s">
-        <v>90</v>
+      <c r="B22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J22" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K22" t="e">
         <v>#N/A</v>
@@ -1270,40 +1507,40 @@
       <c r="L22" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M22" t="s">
-        <v>96</v>
+      <c r="M22" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
         <v>33</v>
       </c>
-      <c r="B23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" t="s">
-        <v>60</v>
-      </c>
-      <c r="G23" t="s">
-        <v>67</v>
-      </c>
-      <c r="H23" t="s">
-        <v>75</v>
-      </c>
-      <c r="I23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J23" t="s">
-        <v>91</v>
+      <c r="B23" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C23" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D23" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E23" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F23" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G23" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H23" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I23" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J23" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K23" t="e">
         <v>#N/A</v>
@@ -1311,37 +1548,37 @@
       <c r="L23" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M23" t="s">
-        <v>97</v>
+      <c r="M23" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
         <v>34</v>
       </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" t="s">
-        <v>61</v>
-      </c>
-      <c r="G24" t="s">
-        <v>68</v>
-      </c>
-      <c r="H24" t="s">
-        <v>76</v>
-      </c>
-      <c r="I24" t="s">
-        <v>84</v>
+      <c r="B24" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C24" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D24" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E24" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F24" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G24" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H24" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I24" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J24" t="e">
         <v>#N/A</v>
@@ -1352,40 +1589,40 @@
       <c r="L24" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M24" t="s">
-        <v>98</v>
+      <c r="M24" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
-      <c r="B25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G25" t="s">
-        <v>69</v>
-      </c>
-      <c r="H25" t="s">
-        <v>77</v>
-      </c>
-      <c r="I25" t="s">
-        <v>85</v>
-      </c>
-      <c r="J25" t="s">
-        <v>92</v>
+      <c r="B25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J25" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K25" t="e">
         <v>#N/A</v>
@@ -1393,40 +1630,40 @@
       <c r="L25" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M25" t="s">
-        <v>99</v>
+      <c r="M25" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
         <v>36</v>
       </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" t="s">
-        <v>57</v>
-      </c>
-      <c r="F26" t="s">
-        <v>62</v>
-      </c>
-      <c r="G26" t="s">
-        <v>70</v>
-      </c>
-      <c r="H26" t="s">
-        <v>78</v>
-      </c>
-      <c r="I26" t="s">
-        <v>86</v>
-      </c>
-      <c r="J26" t="s">
-        <v>93</v>
+      <c r="B26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J26" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K26" t="e">
         <v>#N/A</v>
@@ -1434,40 +1671,40 @@
       <c r="L26" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M26" t="s">
-        <v>100</v>
+      <c r="M26" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
         <v>37</v>
       </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" t="s">
-        <v>71</v>
-      </c>
-      <c r="H27" t="s">
-        <v>79</v>
-      </c>
-      <c r="I27" t="s">
-        <v>87</v>
-      </c>
-      <c r="J27" t="s">
-        <v>94</v>
+      <c r="B27" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C27" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D27" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E27" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F27" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G27" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H27" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I27" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J27" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K27" t="e">
         <v>#N/A</v>
@@ -1475,37 +1712,37 @@
       <c r="L27" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M27" t="s">
-        <v>101</v>
+      <c r="M27" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
         <v>38</v>
       </c>
-      <c r="B28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" t="s">
-        <v>57</v>
-      </c>
-      <c r="F28" t="s">
-        <v>64</v>
-      </c>
-      <c r="G28" t="s">
-        <v>72</v>
-      </c>
-      <c r="H28" t="s">
-        <v>80</v>
-      </c>
-      <c r="I28" t="s">
-        <v>88</v>
+      <c r="B28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I28" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J28" t="e">
         <v>#N/A</v>
@@ -1516,49 +1753,828 @@
       <c r="L28" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M28" t="s">
-        <v>102</v>
+      <c r="M28" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
         <v>39</v>
       </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M29" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M30" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M31" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M32" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M33" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M34" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" t="s">
+        <v>97</v>
+      </c>
+      <c r="F35" t="s">
+        <v>103</v>
+      </c>
+      <c r="G35" t="s">
+        <v>116</v>
+      </c>
+      <c r="H35" t="s">
+        <v>130</v>
+      </c>
+      <c r="I35" t="s">
+        <v>144</v>
+      </c>
+      <c r="J35" t="s">
+        <v>158</v>
+      </c>
+      <c r="K35" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L35" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M35" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" t="s">
+        <v>88</v>
+      </c>
+      <c r="E36" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" t="s">
+        <v>104</v>
+      </c>
+      <c r="G36" t="s">
+        <v>117</v>
+      </c>
+      <c r="H36" t="s">
+        <v>131</v>
+      </c>
+      <c r="I36" t="s">
+        <v>145</v>
+      </c>
+      <c r="J36" t="s">
+        <v>159</v>
+      </c>
+      <c r="K36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M36" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
         <v>47</v>
       </c>
-      <c r="D29" t="s">
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" t="s">
+        <v>105</v>
+      </c>
+      <c r="G37" t="s">
+        <v>118</v>
+      </c>
+      <c r="H37" t="s">
+        <v>132</v>
+      </c>
+      <c r="I37" t="s">
+        <v>146</v>
+      </c>
+      <c r="J37" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K37" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L37" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M37" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" t="s">
+        <v>90</v>
+      </c>
+      <c r="E38" t="s">
+        <v>97</v>
+      </c>
+      <c r="F38" t="s">
+        <v>106</v>
+      </c>
+      <c r="G38" t="s">
+        <v>119</v>
+      </c>
+      <c r="H38" t="s">
+        <v>133</v>
+      </c>
+      <c r="I38" t="s">
+        <v>147</v>
+      </c>
+      <c r="J38" t="s">
+        <v>160</v>
+      </c>
+      <c r="K38" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L38" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M38" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" t="s">
+        <v>91</v>
+      </c>
+      <c r="E39" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39" t="s">
+        <v>120</v>
+      </c>
+      <c r="H39" t="s">
+        <v>134</v>
+      </c>
+      <c r="I39" t="s">
+        <v>148</v>
+      </c>
+      <c r="J39" t="s">
+        <v>161</v>
+      </c>
+      <c r="K39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M39" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" t="s">
+        <v>100</v>
+      </c>
+      <c r="F40" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" t="s">
+        <v>121</v>
+      </c>
+      <c r="H40" t="s">
+        <v>135</v>
+      </c>
+      <c r="I40" t="s">
+        <v>149</v>
+      </c>
+      <c r="J40" t="s">
+        <v>162</v>
+      </c>
+      <c r="K40" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L40" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M40" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" t="s">
+        <v>88</v>
+      </c>
+      <c r="E41" t="s">
+        <v>99</v>
+      </c>
+      <c r="F41" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" t="s">
+        <v>122</v>
+      </c>
+      <c r="H41" t="s">
+        <v>136</v>
+      </c>
+      <c r="I41" t="s">
+        <v>150</v>
+      </c>
+      <c r="J41" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K41" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L41" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M41" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" t="s">
+        <v>97</v>
+      </c>
+      <c r="F42" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42" t="s">
+        <v>123</v>
+      </c>
+      <c r="H42" t="s">
+        <v>137</v>
+      </c>
+      <c r="I42" t="s">
+        <v>151</v>
+      </c>
+      <c r="J42" t="s">
+        <v>163</v>
+      </c>
+      <c r="K42" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L42" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M42" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" t="s">
+        <v>101</v>
+      </c>
+      <c r="F43" t="s">
+        <v>110</v>
+      </c>
+      <c r="G43" t="s">
+        <v>124</v>
+      </c>
+      <c r="H43" t="s">
+        <v>138</v>
+      </c>
+      <c r="I43" t="s">
+        <v>152</v>
+      </c>
+      <c r="J43" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K43" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L43" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M43" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
         <v>54</v>
       </c>
-      <c r="E29" t="s">
+      <c r="B44" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" t="s">
+        <v>92</v>
+      </c>
+      <c r="E44" t="s">
+        <v>98</v>
+      </c>
+      <c r="F44" t="s">
+        <v>111</v>
+      </c>
+      <c r="G44" t="s">
+        <v>125</v>
+      </c>
+      <c r="H44" t="s">
+        <v>139</v>
+      </c>
+      <c r="I44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J44" t="s">
+        <v>164</v>
+      </c>
+      <c r="K44" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L44" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M44" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
         <v>55</v>
       </c>
-      <c r="F29" t="s">
-        <v>65</v>
-      </c>
-      <c r="G29" t="s">
-        <v>73</v>
-      </c>
-      <c r="H29" t="s">
-        <v>81</v>
-      </c>
-      <c r="I29" t="s">
-        <v>89</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="B45" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" t="s">
+        <v>88</v>
+      </c>
+      <c r="E45" t="s">
+        <v>100</v>
+      </c>
+      <c r="F45" t="s">
+        <v>112</v>
+      </c>
+      <c r="G45" t="s">
+        <v>126</v>
+      </c>
+      <c r="H45" t="s">
+        <v>140</v>
+      </c>
+      <c r="I45" t="s">
+        <v>154</v>
+      </c>
+      <c r="J45" t="s">
+        <v>165</v>
+      </c>
+      <c r="K45" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L45" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M45" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" t="s">
+        <v>94</v>
+      </c>
+      <c r="E46" t="s">
+        <v>102</v>
+      </c>
+      <c r="F46" t="s">
+        <v>113</v>
+      </c>
+      <c r="G46" t="s">
+        <v>127</v>
+      </c>
+      <c r="H46" t="s">
+        <v>141</v>
+      </c>
+      <c r="I46" t="s">
+        <v>155</v>
+      </c>
+      <c r="J46" t="s">
+        <v>166</v>
+      </c>
+      <c r="K46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M46" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" t="s">
         <v>95</v>
       </c>
-      <c r="K29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M29" t="s">
-        <v>103</v>
+      <c r="E47" t="s">
+        <v>97</v>
+      </c>
+      <c r="F47" t="s">
+        <v>114</v>
+      </c>
+      <c r="G47" t="s">
+        <v>128</v>
+      </c>
+      <c r="H47" t="s">
+        <v>142</v>
+      </c>
+      <c r="I47" t="s">
+        <v>156</v>
+      </c>
+      <c r="J47" t="s">
+        <v>167</v>
+      </c>
+      <c r="K47" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L47" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M47" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" t="s">
+        <v>96</v>
+      </c>
+      <c r="E48" t="s">
+        <v>100</v>
+      </c>
+      <c r="F48" t="s">
+        <v>115</v>
+      </c>
+      <c r="G48" t="s">
+        <v>129</v>
+      </c>
+      <c r="H48" t="s">
+        <v>143</v>
+      </c>
+      <c r="I48" t="s">
+        <v>157</v>
+      </c>
+      <c r="J48" t="s">
+        <v>168</v>
+      </c>
+      <c r="K48" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L48" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M48" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>